<commit_message>
Update source data and widget def for homelessness npa.  Uploader lagging.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Description" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Progress" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Description" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -59,6 +60,30 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">NSW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aust</t>
   </si>
   <si>
@@ -74,6 +99,9 @@
     <t xml:space="preserve">Need for services met</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A </t>
+  </si>
+  <si>
     <t xml:space="preserve">Clients experiencing family and domestic violence</t>
   </si>
   <si>
@@ -84,6 +112,33 @@
   </si>
   <si>
     <t xml:space="preserve">2014-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 30a. National Partnership Agreement on Homelessness 2015-17 outcomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone/Performance Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 1 of project plans submitted to the Commonwealth (1 July 2015) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not applicable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 2 of project plans submitted to the Commonwealth (1 September 2015) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Commonwealth on assessment of progress against project plans, and provide assurance funding has been matched (1 September 2016) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In progress </t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 25 per cent of total matched funding directed to addressing priority outputs</t>
   </si>
   <si>
     <t xml:space="preserve">Updated</t>
@@ -120,10 +175,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -163,7 +220,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -216,7 +286,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,16 +295,48 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -255,21 +357,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="19" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.6173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -285,155 +385,470 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>67</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>97</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>77</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>93</v>
+      </c>
+      <c r="L5" s="6" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="6" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="s">
-        <v>6</v>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>34</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>22</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>31.9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5" t="n">
         <v>76</v>
       </c>
+      <c r="G10" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>91</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="0" t="n">
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="6" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>33</v>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>39</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>31</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>29</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>38</v>
+      </c>
+      <c r="L12" s="7" t="n">
+        <v>33.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="0" t="n">
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="0" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="0" t="n">
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>77</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>73</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="L15" s="6" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="6" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="0" t="n">
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="7" t="n">
         <v>36</v>
       </c>
+      <c r="E17" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <v>31</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <v>43</v>
+      </c>
+      <c r="L17" s="7" t="n">
+        <v>36.1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <v>16</v>
       </c>
     </row>
@@ -443,7 +858,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -456,71 +871,270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="60.1632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.280612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.1836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="n">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
-        <v>15</v>
+      <c r="B4" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
-        <v>16</v>
+      <c r="B5" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
+      <c r="A7" s="3"/>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Homelessness NPA uploader updated for new widget def.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="37">
   <si>
     <r>
       <rPr>
@@ -117,9 +117,6 @@
     <t xml:space="preserve">Figure 30a. National Partnership Agreement on Homelessness 2015-17 outcomes</t>
   </si>
   <si>
-    <t xml:space="preserve">Milestone/Performance Indicator</t>
-  </si>
-  <si>
     <t xml:space="preserve">Part 1 of project plans submitted to the Commonwealth (1 July 2015) </t>
   </si>
   <si>
@@ -147,7 +144,7 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Improving</t>
+    <t xml:space="preserve">On track</t>
   </si>
   <si>
     <t xml:space="preserve">Desc Body</t>
@@ -359,12 +356,12 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="19" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -413,9 +410,7 @@
       <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -871,188 +866,199 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="8" width="60.1632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.280612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1079,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1085,7 +1091,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>2015</v>
@@ -1093,42 +1099,42 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Newly received state-level youths-reporting-alone data.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="37">
   <si>
     <r>
       <rPr>
@@ -356,17 +356,19 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="19" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -529,32 +531,32 @@
       <c r="C8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>18</v>
+      <c r="D8" s="7" t="n">
+        <v>23.3999961503667</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>17.5090307369514</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>13.1976307472634</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>13.8878383362982</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>23.8159275780635</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>22.8246078922868</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>26.2771546745165</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>15.2998318699795</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>18.4585859859986</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,32 +676,32 @@
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>17</v>
+      <c r="D13" s="7" t="n">
+        <v>23.4988790471611</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>15.5294407371146</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>12.4667434652623</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>14.1770226899537</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>24.4880995261977</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>21.7135600139093</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <v>22.9096018735363</v>
+      </c>
+      <c r="K13" s="7" t="n">
+        <v>12.8932627648075</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <v>17.4856447698144</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,32 +821,32 @@
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <v>16</v>
+      <c r="D18" s="7" t="n">
+        <v>22.6366303645134</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>14.2867149126349</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>12.0006875759104</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>13.2053916223953</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>24.0283572406151</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>18.4779345541879</v>
+      </c>
+      <c r="J18" s="7" t="n">
+        <v>23.2458339182225</v>
+      </c>
+      <c r="K18" s="7" t="n">
+        <v>11.6582783188444</v>
+      </c>
+      <c r="L18" s="7" t="n">
+        <v>16.3422284440929</v>
       </c>
     </row>
   </sheetData>
@@ -869,21 +871,21 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D8:L8 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="60.1632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="59.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,14 +1081,15 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D8:L8 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Expel weird text block apostrophe.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -162,10 +162,10 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Note (a) NPAH funded agencies were required to participate in the SHSC administered by the Australian Institute of Health and Welfare – although some were granted an exemption by the Commonwealth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(b) The SHSC does not report on NPAH initiatives exclusively, it also includes services funded under the National Affordable Housing Agreement.</t>
+    <t xml:space="preserve">NPAH funded agencies were required to participate in the SHSC administered by the Australian Institute of Health and Welfare – although some were granted an exemption by the Commonwealth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The SHSC does not report on NPAH initiatives exclusively, it also includes services funded under the National Affordable Housing Agreement.</t>
   </si>
 </sst>
 </file>
@@ -356,19 +356,19 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="19" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8:L8"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -871,21 +871,20 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D8:L8 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="59.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="58.719387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,15 +1080,15 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D8:L8 B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,7 +1120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
@@ -1134,7 +1133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="9" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Various bugfixes and tweaks.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -144,7 +144,7 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">On track</t>
+    <t xml:space="preserve">Negative Change</t>
   </si>
   <si>
     <t xml:space="preserve">Desc Body</t>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>